<commit_message>
first step of the algorithm
</commit_message>
<xml_diff>
--- a/2021-11-19 Roder связи.xlsx
+++ b/2021-11-19 Roder связи.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Договор заключен</t>
   </si>
   <si>
-    <t xml:space="preserve">R1080, R1190, R1030, R1870</t>
+    <t xml:space="preserve">R1080, R1190, R1030</t>
   </si>
   <si>
     <t xml:space="preserve">    R1010</t>
@@ -358,7 +358,7 @@
     <t xml:space="preserve">Подъем каркаса</t>
   </si>
   <si>
-    <t xml:space="preserve">R1000, R1840, R1850, R1860, R1830, R1820</t>
+    <t xml:space="preserve">R1840, R1850, R1860, R1830, R1820</t>
   </si>
   <si>
     <t xml:space="preserve">R1220, R1040, R1790, R1280, R1800, R1810, R1200, R1770</t>
@@ -1229,20 +1229,20 @@
   </sheetPr>
   <dimension ref="A1:N116"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A116" activeCellId="0" sqref="A116"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="87.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="73.85"/>
   </cols>
   <sheetData>

</xml_diff>